<commit_message>
Added formal German and Italian
</commit_message>
<xml_diff>
--- a/data_raw/RAT_dict.xlsx
+++ b/data_raw/RAT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\RAT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A1A8C3C-0761-4735-9DC6-FB3CBA2950E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E3CF3-0000-4D69-AF5D-6786214B8D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAT_dict" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
   <si>
     <t>key</t>
   </si>
@@ -46,9 +46,6 @@
     <t>In this test you will hear a number of short rhythms which you have to match to a corresponding image. The rhythms will be preceeded and followed by four metronome clicks each. First you'll hear a few examples and do some practice questions.</t>
   </si>
   <si>
-    <t>In diesem Test hörst du einige kurze Rhythmen, die du zu dem dazugehörigen Bild zuordnen sollst. Die Rhythmen werden von jeweils vier Metronomklicks umrahmt. Zunächst hörst du einige Beispiele und machst ein paar Übungsaufgaben.</t>
-  </si>
-  <si>
     <t>SAMPLE1a</t>
   </si>
   <si>
@@ -359,12 +356,180 @@
   </si>
   <si>
     <t>Du hast den  Rhythmuswahrnehmungstest beendet.</t>
+  </si>
+  <si>
+    <t>DE_F</t>
+  </si>
+  <si>
+    <t>**Beispiel 1**\\Jeder Rhythmus besteht aus Bassdrum und Claps.\\Die Claps werden als hellblaue Quadrate in der oberen Reihe dargestellt und die Bassdrumschläge als dunkelblaue Quadrate in der unteren Reihe.\\Klicken Sie auf das Abspielzeichen, um den Rhythmus zu hören. Vor und nach dem Rhythmus werden 4 Metronomklicks zu hören sein.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}**\\Klicke Sie auf  'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen,\\ oder klicken Sie auf 'Weiter', um zum  Haupttest zu gelangen.</t>
+  </si>
+  <si>
+    <t>Nun geht es mit dem Haupttest los, in dem Ihre  Ergebnisse gespeichert werden.\\Ab jetzt bekommen Sie keine Rückmeldung mehr. Viel Erfolg!</t>
+  </si>
+  <si>
+    <t>Ihr Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
+  </si>
+  <si>
+    <t>Nur eins der Bilder passt zu dem Rhythmus. Welches? Wenn Sie nicht sicher sind, dann entscheiden Sie aus dem Bauch heraus.</t>
+  </si>
+  <si>
+    <t>Sie haben den Rhythmus-Wahrnehmungs-Test abgeschlossen.\\Von {{num_question}} Aufgaben waren {{num_correct}} richtig.</t>
+  </si>
+  <si>
+    <t>Im Vergleich zu anderen, die an dem Test teilgenommen haben, ist Ihr Rhythmus IQ:</t>
+  </si>
+  <si>
+    <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und Sie hören jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Ihre Aufgabe ist es, den Rhythmus zu hören und dann auf das Bild der vier Bilder klicken, das mit dem Rhyhtmus übereinstimmt, den Sie gerade gehört haben.\\ Lassen Sie uns das mal üben.</t>
+  </si>
+  <si>
+    <t>Klicken Sie hier, falls das Audio nicht spielt.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie Ihre ID ein</t>
+  </si>
+  <si>
+    <t>Ihre Ergebnisse wurden gespeichert.</t>
+  </si>
+  <si>
+    <t>Sie können den Browsertab jetzt schließen.</t>
+  </si>
+  <si>
+    <t>Ihr Testergebnis</t>
+  </si>
+  <si>
+    <t>Sie haben den  Rhythmuswahrnehmungstest beendet.</t>
+  </si>
+  <si>
+    <t>In diesem Test hören Sie einige kurze Rhythmen, die Sie dem dazugehörigen Bild zuordnen sollen. Die Rhythmen werden von jeweils vier Metronomklicks umrahmt. Zunächst hören Sie einige Beispiele und machen ein paar Übungsaufgaben.</t>
+  </si>
+  <si>
+    <t>In diesem Test hörst du einige kurze Rhythmen, die du dem dazugehörigen Bild zuordnen sollst. Die Rhythmen werden von jeweils vier Metronomklicks umrahmt. Zunächst hörst du einige Beispiele und machst ein paar Übungsaufgaben.</t>
+  </si>
+  <si>
+    <t>Welches Bild passt zu dem Rhythmus, den Sie  gerade gehört haben? Klicke Sie auf das richtige. Wenn Sie sich nicht sicher sind, dann entscheiden Sie aus dem Bauch heraus.</t>
+  </si>
+  <si>
+    <t>Welches Bild passt zu dem Rhythmus, den Sie gerade gehört haben? Klicken Sie auf das richtige. Wenn Sie sich nicht sicher sind, dann entscheiden Sie aus dem Bauch heraus.</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Benvenuto/a al test sul ritmo musicale!</t>
+  </si>
+  <si>
+    <t>**Applauso** **Applauso** Grancassa Grancassa</t>
+  </si>
+  <si>
+    <t>**Esempio 2**\\Ecco qui un altro ritmo:</t>
+  </si>
+  <si>
+    <t>Debole **Forte** Debole **Forte**</t>
+  </si>
+  <si>
+    <t>IQ di Percezione Ritmica</t>
+  </si>
+  <si>
+    <t>**Esercitazione  1** \\ Ecco un esempio pratico di quattro suoni</t>
+  </si>
+  <si>
+    <t>Quale immagine corrisponde al ritmo che hai appena sentito? Clicca su quella corretta. Se non lo sai, prova a fare del tuo meglio!</t>
+  </si>
+  <si>
+    <t>Il primo</t>
+  </si>
+  <si>
+    <t>Giusto!</t>
+  </si>
+  <si>
+    <t>**Esercitazione 2**\\**{{feedback}}**\\ Proviamo con un esempio pratico di 8 suoni</t>
+  </si>
+  <si>
+    <t>Sbagliato.</t>
+  </si>
+  <si>
+    <t>Premi "Indietro" per leggere le istruzioni e ripeti le prove di esercitazione,\\oppure premi "Continua" per procedere con il test principale.</t>
+  </si>
+  <si>
+    <t>Il secondo</t>
+  </si>
+  <si>
+    <t>Stai per iniziare il test principale, in cui i tuoi risultati verranno registrati\\Potrai ascoltare ogni ritmo solo una volta\\ Non riceverai i risultati dopo le singole domande. Buona fortuna!</t>
+  </si>
+  <si>
+    <t>Domanda {{num_question}} di {{test_length}}</t>
+  </si>
+  <si>
+    <t>Solo una di queste immagini corrisponde al ritmo. Quale? Se non lo sai, prova a fare del tuo meglio!</t>
+  </si>
+  <si>
+    <t>Hai completato il test di percezione ritmica!\\Hai risposto correttamente a {{num_correct}} su {{num_question}}.</t>
+  </si>
+  <si>
+    <t>Continua</t>
+  </si>
+  <si>
+    <t>Indietro</t>
+  </si>
+  <si>
+    <t>IQ Ritmico</t>
+  </si>
+  <si>
+    <t>**Esercitazione 3**\\**{{feedback}}**\\ Proviamo con un esempio pratico finale di 16 suoni.</t>
+  </si>
+  <si>
+    <t>Per favore inserisci il tuo codice partecipante</t>
+  </si>
+  <si>
+    <t>es. 123456</t>
+  </si>
+  <si>
+    <t>I tuoi risultati sono stati salvati</t>
+  </si>
+  <si>
+    <t>Adesso puoi chiudere la finestra del browser</t>
+  </si>
+  <si>
+    <t>Il codice partecipante deve iniziare con UK o AUS seguito da un underscore e un numero, es. UK_01 o AUS_02</t>
+  </si>
+  <si>
+    <t>Il tuo punteggio</t>
+  </si>
+  <si>
+    <t>Punteggio</t>
+  </si>
+  <si>
+    <t>Test sul Ritmo Musicale</t>
+  </si>
+  <si>
+    <t>Hai completato il test sul ritmo musicale.</t>
+  </si>
+  <si>
+    <t>In questo test ascolterai una serie di brevi sequenze ritmiche che dovrai abbinare a un'immagine corrispondente. Ciascuno dei ritmi sarà preceduto e seguito da quattro click di metronomo. Per prima cosa ascolterai alcuni esempi e farai alcune prove per esercitarti.</t>
+  </si>
+  <si>
+    <t>**Esempio 1** Ogni ritmo è composto da suoni di applausi e grancassa \\ Gli applausi sono rappresentati da quadrati azzurri nella riga superiore e la grancassa da quadrati blu scuri nella riga inferiore\\ Ascolta questo breve ritmo facendo click sul pulsante Play. Sentirai 4 click di metronomo prima e dopo il ritmo.</t>
+  </si>
+  <si>
+    <t>Il tuo browser non supporta l’audio. Questo test non può funzionare senz’audio, ci dispiace!</t>
+  </si>
+  <si>
+    <t>Rispetto alla popolazione generale il tuo QI ritmico è</t>
+  </si>
+  <si>
+    <t>Le sequenze ritmiche saranno composte da quattro, otto o sedici suoni e ci saranno quattro click di metronomo prima e dopo il ritmo effettivo \\ Il tuo compito è ascoltare il ritmo e quindi cliccare sull'immagine tra le quattro opzioni che corrisponde al ritmo che hai appena sentito\\Facciamo un po’ di pratica.</t>
+  </si>
+  <si>
+    <t>Clicca qui se l’audio non parte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -842,8 +1007,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1198,16 +1366,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,8 +1385,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1228,8 +1402,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1237,392 +1417,608 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>75</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>87</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>93</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>96</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>99</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>101</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>102</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>104</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>107</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>108</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="C38" t="s">
-        <v>112</v>
+      <c r="D38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added de_f, version 0.1.5
</commit_message>
<xml_diff>
--- a/data_raw/RAT_dict.xlsx
+++ b/data_raw/RAT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\RAT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E3CF3-0000-4D69-AF5D-6786214B8D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2CAF1D-82A9-40CC-9824-15EDA37B758F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="169">
   <si>
     <t>key</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Ihr Testergebnis</t>
   </si>
   <si>
-    <t>Sie haben den  Rhythmuswahrnehmungstest beendet.</t>
-  </si>
-  <si>
     <t>In diesem Test hören Sie einige kurze Rhythmen, die Sie dem dazugehörigen Bild zuordnen sollen. Die Rhythmen werden von jeweils vier Metronomklicks umrahmt. Zunächst hören Sie einige Beispiele und machen ein paar Übungsaufgaben.</t>
   </si>
   <si>
@@ -524,6 +521,12 @@
   </si>
   <si>
     <t>Clicca qui se l’audio non parte</t>
+  </si>
+  <si>
+    <t>Der Rhythmuswahrnehmungstest ist beendet.</t>
+  </si>
+  <si>
+    <t>Test: Rhythmuswahrnehmung</t>
   </si>
 </sst>
 </file>
@@ -1369,11 +1372,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1389,7 +1395,7 @@
         <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1403,10 +1409,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,13 +1423,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,7 +1446,7 @@
         <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1457,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1491,7 +1497,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1508,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1525,7 +1531,7 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,10 +1545,10 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,7 +1565,7 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,7 +1582,7 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1599,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1610,7 +1616,7 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1627,7 +1633,7 @@
         <v>114</v>
       </c>
       <c r="E15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,7 +1650,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,7 +1667,7 @@
         <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1678,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,7 +1701,7 @@
         <v>116</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1712,7 +1718,7 @@
         <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,7 +1735,7 @@
         <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,7 +1752,7 @@
         <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1760,10 +1766,10 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,7 +1786,7 @@
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,7 +1803,7 @@
         <v>119</v>
       </c>
       <c r="E25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1814,7 +1820,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1831,7 +1837,7 @@
         <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,7 +1854,7 @@
         <v>120</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1865,7 +1871,7 @@
         <v>121</v>
       </c>
       <c r="E29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,7 +1888,7 @@
         <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1899,7 +1905,7 @@
         <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,7 +1922,7 @@
         <v>123</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,7 +1939,7 @@
         <v>124</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1950,7 +1956,7 @@
         <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1967,7 +1973,7 @@
         <v>125</v>
       </c>
       <c r="E35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1984,7 +1990,7 @@
         <v>105</v>
       </c>
       <c r="E36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,7 +2007,7 @@
         <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2015,10 +2021,10 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some typos in German language
</commit_message>
<xml_diff>
--- a/data_raw/RAT_dict.xlsx
+++ b/data_raw/RAT_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\RAT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2CAF1D-82A9-40CC-9824-15EDA37B758F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17EA542-F263-45D7-B54C-FCA6AE9C4C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,9 +265,6 @@
     <t>The rhythms will all have four, eight or sixteen sounds and four clicks of a metronome before and after the actual rhythm.\\Your task is to listen to the rhythm and then click on the one image from among four options that corresponds to the rhythm that you just heard. \\Let's have some practice.</t>
   </si>
   <si>
-    <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und du hörst jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Deine Aufgabe ist es, den Rhythmus zu hören und dann auf das Bild der vier Bilder klicken, das mit dem Rhyhtmus übereinstimmt, den du gerade gehört hast.\\ Lass uns das mal üben.</t>
-  </si>
-  <si>
     <t>CLICK_TO_PLAY</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>Im Vergleich zu anderen, die an dem Test teilgenommen haben, ist Ihr Rhythmus IQ:</t>
   </si>
   <si>
-    <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und Sie hören jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Ihre Aufgabe ist es, den Rhythmus zu hören und dann auf das Bild der vier Bilder klicken, das mit dem Rhyhtmus übereinstimmt, den Sie gerade gehört haben.\\ Lassen Sie uns das mal üben.</t>
-  </si>
-  <si>
     <t>Klicken Sie hier, falls das Audio nicht spielt.</t>
   </si>
   <si>
@@ -527,6 +521,12 @@
   </si>
   <si>
     <t>Test: Rhythmuswahrnehmung</t>
+  </si>
+  <si>
+    <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und du hörst jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Deine Aufgabe ist es, den Rhythmus zu hören und dann auf dasjenige Bild der vier Bilder zu klicken, das mit dem Rhythmus übereinstimmt, den du gerade gehört hast.\\ Lass uns das mal üben.</t>
+  </si>
+  <si>
+    <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und Sie hören jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Ihre Aufgabe ist es, den Rhythmus zu hören und dann auf dasjenige Bild der vier Bilder zu klicken, das mit dem Rhythmus übereinstimmt, den Sie gerade gehört haben.\\ Lassen Sie uns das mal üben.</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,10 +1392,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,13 +1423,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,10 +1443,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,10 +1545,10 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,7 +1565,7 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,10 +1630,10 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1664,10 +1664,10 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,10 +1698,10 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1715,10 +1715,10 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,10 +1732,10 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,10 +1766,10 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,7 +1786,7 @@
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,10 +1800,10 @@
         <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,183 +1848,183 @@
         <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="E28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" t="s">
-        <v>87</v>
-      </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" t="s">
-        <v>90</v>
-      </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" t="s">
-        <v>93</v>
-      </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
         <v>94</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>95</v>
       </c>
-      <c r="C33" t="s">
-        <v>96</v>
-      </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
         <v>97</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
         <v>100</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="C35" t="s">
-        <v>102</v>
-      </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
         <v>103</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="C36" t="s">
-        <v>105</v>
-      </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>107</v>
       </c>
-      <c r="C37" t="s">
-        <v>108</v>
-      </c>
       <c r="D37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
         <v>109</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>110</v>
       </c>
-      <c r="C38" t="s">
-        <v>111</v>
-      </c>
       <c r="D38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed practice feedback in German
</commit_message>
<xml_diff>
--- a/data_raw/RAT_dict.xlsx
+++ b/data_raw/RAT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\RAT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17EA542-F263-45D7-B54C-FCA6AE9C4C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD18CC0-28E7-4C5D-9AEA-8C102C9167EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAT_dict" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>Incorrect.</t>
   </si>
   <si>
-    <t>Falsch.</t>
-  </si>
-  <si>
     <t>TRANSITION</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>Der Rhythmus wird aus vier, acht oder sechzehn Klängen/Tönen bestehen und Sie hören jeweils vier Metronomschläge vor und nach dem Rhythmus.\\Ihre Aufgabe ist es, den Rhythmus zu hören und dann auf dasjenige Bild der vier Bilder zu klicken, das mit dem Rhythmus übereinstimmt, den Sie gerade gehört haben.\\ Lassen Sie uns das mal üben.</t>
+  </si>
+  <si>
+    <t>Leider falsch.</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,10 +1392,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,13 +1423,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,10 +1443,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,10 +1545,10 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,7 +1565,7 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1610,421 +1610,421 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
       <c r="C28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" t="s">
         <v>167</v>
       </c>
-      <c r="D28" t="s">
-        <v>168</v>
-      </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
-        <v>95</v>
-      </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
-        <v>101</v>
-      </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
         <v>105</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>106</v>
       </c>
-      <c r="C37" t="s">
-        <v>107</v>
-      </c>
       <c r="D37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
         <v>108</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>109</v>
       </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>